<commit_message>
updates for the revision, mainly related to results and file structure
</commit_message>
<xml_diff>
--- a/multiverse/data/pipelines_multiverse.xlsx
+++ b/multiverse/data/pipelines_multiverse.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="62">
   <si>
     <t xml:space="preserve">Pipelines</t>
   </si>
@@ -142,6 +142,9 @@
     <t xml:space="preserve">Compute_connectivity</t>
   </si>
   <si>
+    <t xml:space="preserve">Connectivity_normalization</t>
+  </si>
+  <si>
     <t xml:space="preserve">Graph_characteristics</t>
   </si>
   <si>
@@ -157,12 +160,21 @@
     <t xml:space="preserve">Pipeline 3</t>
   </si>
   <si>
+    <t xml:space="preserve">F-Global_signal</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pipeline 4</t>
   </si>
   <si>
     <t xml:space="preserve">Pipeline 5</t>
   </si>
   <si>
+    <t xml:space="preserve">F-motion_regression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F-Other_confound_regression</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pipeline 6</t>
   </si>
   <si>
@@ -181,19 +193,10 @@
     <t xml:space="preserve">Pipeline 11</t>
   </si>
   <si>
-    <t xml:space="preserve">F-Global_signal</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pipeline 12</t>
   </si>
   <si>
     <t xml:space="preserve">Pipeline 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F-motion_regression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F-Other_confound_regression</t>
   </si>
   <si>
     <t xml:space="preserve">Pipeline 14</t>
@@ -212,7 +215,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -241,31 +244,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFE699"/>
-        <bgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -302,32 +287,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -340,66 +321,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFE699"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -580,14 +501,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BI31"/>
+  <dimension ref="A1:AMJ33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="14" topLeftCell="R15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="14" topLeftCell="Q15" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="R1" activeCellId="0" sqref="R1"/>
+      <selection pane="topRight" activeCell="Q1" activeCellId="0" sqref="Q1"/>
       <selection pane="bottomLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="W22" activeCellId="0" sqref="W22"/>
+      <selection pane="bottomRight" activeCell="U22" activeCellId="0" sqref="U22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.890625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -688,7 +609,13 @@
       <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="0"/>
+      <c r="X1" s="2"/>
+      <c r="AME1" s="2"/>
+      <c r="AMF1" s="2"/>
+      <c r="AMG1" s="2"/>
+      <c r="AMH1" s="2"/>
+      <c r="AMI1" s="2"/>
+      <c r="AMJ1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -697,37 +624,37 @@
       <c r="B2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="3" t="s">
         <v>35</v>
       </c>
       <c r="N2" s="1" t="s">
@@ -739,95 +666,98 @@
       <c r="P2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="U2" s="0"/>
-      <c r="V2" s="0"/>
-      <c r="W2" s="0"/>
-      <c r="X2" s="0"/>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
-      <c r="AD2" s="2"/>
-      <c r="AE2" s="2"/>
-      <c r="AF2" s="2"/>
-      <c r="AG2" s="2"/>
-      <c r="AH2" s="2"/>
-      <c r="AI2" s="2"/>
-      <c r="AJ2" s="2"/>
-      <c r="AK2" s="2"/>
-      <c r="AL2" s="2"/>
-      <c r="AM2" s="2"/>
-      <c r="AN2" s="2"/>
-      <c r="AO2" s="2"/>
-      <c r="AP2" s="5"/>
-      <c r="AQ2" s="6"/>
-      <c r="AR2" s="6"/>
-      <c r="AS2" s="6"/>
-      <c r="AT2" s="6"/>
-      <c r="AU2" s="2"/>
-      <c r="AV2" s="2"/>
-      <c r="AW2" s="2"/>
-      <c r="AX2" s="2"/>
-      <c r="AY2" s="2"/>
-      <c r="AZ2" s="2"/>
-      <c r="BA2" s="2"/>
-      <c r="BB2" s="2"/>
-      <c r="BC2" s="2"/>
-      <c r="BD2" s="2"/>
-      <c r="BE2" s="6"/>
-      <c r="BF2" s="6"/>
-      <c r="BG2" s="6"/>
-      <c r="BH2" s="6"/>
-      <c r="BI2" s="6"/>
+      <c r="U2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="3"/>
+      <c r="AH2" s="3"/>
+      <c r="AI2" s="3"/>
+      <c r="AJ2" s="3"/>
+      <c r="AK2" s="3"/>
+      <c r="AL2" s="3"/>
+      <c r="AM2" s="3"/>
+      <c r="AN2" s="3"/>
+      <c r="AO2" s="3"/>
+      <c r="AP2" s="3"/>
+      <c r="AQ2" s="3"/>
+      <c r="AR2" s="3"/>
+      <c r="AS2" s="3"/>
+      <c r="AT2" s="3"/>
+      <c r="AU2" s="3"/>
+      <c r="AV2" s="3"/>
+      <c r="ALW2" s="2"/>
+      <c r="ALX2" s="2"/>
+      <c r="ALY2" s="2"/>
+      <c r="ALZ2" s="2"/>
+      <c r="AMA2" s="2"/>
+      <c r="AMB2" s="2"/>
+      <c r="AMC2" s="2"/>
+      <c r="AMD2" s="2"/>
+      <c r="AME2" s="2"/>
+      <c r="AMF2" s="2"/>
+      <c r="AMG2" s="2"/>
+      <c r="AMH2" s="2"/>
+      <c r="AMI2" s="2"/>
+      <c r="AMJ2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="3" t="s">
         <v>35</v>
       </c>
       <c r="N3" s="1" t="s">
@@ -836,96 +766,100 @@
       <c r="O3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="P3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="Q3" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="R3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="S3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="T3" s="0"/>
-      <c r="U3" s="0"/>
-      <c r="V3" s="0"/>
-      <c r="W3" s="0"/>
-      <c r="X3" s="0"/>
-      <c r="AB3" s="2"/>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="2"/>
-      <c r="AE3" s="2"/>
-      <c r="AF3" s="2"/>
-      <c r="AG3" s="2"/>
-      <c r="AH3" s="2"/>
-      <c r="AI3" s="2"/>
-      <c r="AJ3" s="2"/>
-      <c r="AK3" s="2"/>
-      <c r="AL3" s="2"/>
-      <c r="AM3" s="2"/>
-      <c r="AN3" s="2"/>
-      <c r="AO3" s="2"/>
-      <c r="AP3" s="5"/>
-      <c r="AQ3" s="6"/>
-      <c r="AR3" s="6"/>
-      <c r="AS3" s="6"/>
-      <c r="AT3" s="6"/>
-      <c r="AU3" s="2"/>
-      <c r="AV3" s="2"/>
-      <c r="AW3" s="2"/>
-      <c r="AX3" s="2"/>
-      <c r="AY3" s="2"/>
-      <c r="AZ3" s="2"/>
-      <c r="BA3" s="2"/>
-      <c r="BB3" s="2"/>
-      <c r="BC3" s="2"/>
-      <c r="BD3" s="2"/>
-      <c r="BE3" s="6"/>
-      <c r="BF3" s="6"/>
-      <c r="BG3" s="6"/>
-      <c r="BH3" s="6"/>
-      <c r="BI3" s="6"/>
+      <c r="T3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3"/>
+      <c r="AG3" s="3"/>
+      <c r="AH3" s="3"/>
+      <c r="AI3" s="3"/>
+      <c r="AJ3" s="3"/>
+      <c r="AK3" s="3"/>
+      <c r="AL3" s="3"/>
+      <c r="AM3" s="3"/>
+      <c r="AN3" s="3"/>
+      <c r="AO3" s="3"/>
+      <c r="AP3" s="3"/>
+      <c r="AQ3" s="3"/>
+      <c r="AR3" s="3"/>
+      <c r="AS3" s="3"/>
+      <c r="AT3" s="3"/>
+      <c r="AU3" s="3"/>
+      <c r="AV3" s="3"/>
+      <c r="ALV3" s="2"/>
+      <c r="ALW3" s="2"/>
+      <c r="ALX3" s="2"/>
+      <c r="ALY3" s="2"/>
+      <c r="ALZ3" s="2"/>
+      <c r="AMA3" s="2"/>
+      <c r="AMB3" s="2"/>
+      <c r="AMC3" s="2"/>
+      <c r="AMD3" s="2"/>
+      <c r="AME3" s="2"/>
+      <c r="AMF3" s="2"/>
+      <c r="AMG3" s="2"/>
+      <c r="AMH3" s="2"/>
+      <c r="AMI3" s="2"/>
+      <c r="AMJ3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" s="3" t="s">
         <v>35</v>
       </c>
       <c r="N4" s="1" t="s">
@@ -934,64 +868,82 @@
       <c r="O4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="P4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="R4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="S4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="T4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="T4" s="4" t="s">
+      <c r="U4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="U4" s="0"/>
-      <c r="V4" s="0"/>
-      <c r="W4" s="0"/>
-      <c r="X4" s="0"/>
+      <c r="V4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="ALW4" s="2"/>
+      <c r="ALX4" s="2"/>
+      <c r="ALY4" s="2"/>
+      <c r="ALZ4" s="2"/>
+      <c r="AMA4" s="2"/>
+      <c r="AMB4" s="2"/>
+      <c r="AMC4" s="2"/>
+      <c r="AMD4" s="2"/>
+      <c r="AME4" s="2"/>
+      <c r="AMF4" s="2"/>
+      <c r="AMG4" s="2"/>
+      <c r="AMH4" s="2"/>
+      <c r="AMI4" s="2"/>
+      <c r="AMJ4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="3" t="s">
         <v>35</v>
       </c>
       <c r="N5" s="1" t="s">
@@ -1000,62 +952,80 @@
       <c r="O5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="P5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="R5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="S5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="S5" s="4" t="s">
+      <c r="T5" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="T5" s="0"/>
-      <c r="U5" s="0"/>
-      <c r="V5" s="0"/>
-      <c r="W5" s="0"/>
-      <c r="X5" s="0"/>
+      <c r="U5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="ALW5" s="2"/>
+      <c r="ALX5" s="2"/>
+      <c r="ALY5" s="2"/>
+      <c r="ALZ5" s="2"/>
+      <c r="AMA5" s="2"/>
+      <c r="AMB5" s="2"/>
+      <c r="AMC5" s="2"/>
+      <c r="AMD5" s="2"/>
+      <c r="AME5" s="2"/>
+      <c r="AMF5" s="2"/>
+      <c r="AMG5" s="2"/>
+      <c r="AMH5" s="2"/>
+      <c r="AMI5" s="2"/>
+      <c r="AMJ5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M6" s="3" t="s">
         <v>35</v>
       </c>
       <c r="N6" s="1" t="s">
@@ -1064,64 +1034,84 @@
       <c r="O6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="P6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="R6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Q6" s="4" t="s">
+      <c r="S6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="R6" s="4" t="s">
+      <c r="T6" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="S6" s="4" t="s">
+      <c r="U6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="T6" s="4" t="s">
+      <c r="V6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="U6" s="0"/>
-      <c r="V6" s="0"/>
-      <c r="W6" s="0"/>
-      <c r="X6" s="0"/>
+      <c r="W6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="X6" s="2"/>
+      <c r="ALW6" s="2"/>
+      <c r="ALX6" s="2"/>
+      <c r="ALY6" s="2"/>
+      <c r="ALZ6" s="2"/>
+      <c r="AMA6" s="2"/>
+      <c r="AMB6" s="2"/>
+      <c r="AMC6" s="2"/>
+      <c r="AMD6" s="2"/>
+      <c r="AME6" s="2"/>
+      <c r="AMF6" s="2"/>
+      <c r="AMG6" s="2"/>
+      <c r="AMH6" s="2"/>
+      <c r="AMI6" s="2"/>
+      <c r="AMJ6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="M7" s="3" t="s">
         <v>35</v>
       </c>
       <c r="N7" s="1" t="s">
@@ -1130,62 +1120,68 @@
       <c r="O7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="P7" s="4" t="s">
+      <c r="P7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="R7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="Q7" s="4" t="s">
+      <c r="S7" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="R7" s="4" t="s">
+      <c r="T7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="S7" s="4" t="s">
+      <c r="U7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="T7" s="0"/>
-      <c r="U7" s="0"/>
-      <c r="V7" s="0"/>
-      <c r="W7" s="0"/>
-      <c r="X7" s="0"/>
+      <c r="V7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="L8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="M8" s="3" t="s">
         <v>35</v>
       </c>
       <c r="N8" s="1" t="s">
@@ -1194,64 +1190,72 @@
       <c r="O8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="P8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="S8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Q8" s="4" t="s">
+      <c r="T8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="R8" s="4" t="s">
+      <c r="U8" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="S8" s="4" t="s">
+      <c r="V8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="T8" s="4" t="s">
+      <c r="W8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="U8" s="0"/>
-      <c r="V8" s="0"/>
-      <c r="W8" s="0"/>
-      <c r="X8" s="0"/>
+      <c r="X8" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="L9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="M9" s="3" t="s">
         <v>35</v>
       </c>
       <c r="N9" s="1" t="s">
@@ -1260,62 +1264,70 @@
       <c r="O9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="P9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="S9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="Q9" s="4" t="s">
+      <c r="T9" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="R9" s="4" t="s">
+      <c r="U9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="S9" s="4" t="s">
+      <c r="V9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="T9" s="0"/>
-      <c r="U9" s="0"/>
-      <c r="V9" s="0"/>
-      <c r="W9" s="0"/>
-      <c r="X9" s="0"/>
+      <c r="W9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="X9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="L10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="M10" s="3" t="s">
         <v>35</v>
       </c>
       <c r="N10" s="1" t="s">
@@ -1327,61 +1339,63 @@
       <c r="P10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Q10" s="4" t="s">
+      <c r="Q10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="R10" s="4" t="s">
+      <c r="R10" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="S10" s="4" t="s">
+      <c r="S10" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="T10" s="4" t="s">
+      <c r="T10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="U10" s="0"/>
-      <c r="V10" s="0"/>
-      <c r="W10" s="0"/>
-      <c r="X10" s="0"/>
+      <c r="U10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="L11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="M11" s="3" t="s">
         <v>35</v>
       </c>
       <c r="N11" s="1" t="s">
@@ -1390,66 +1404,68 @@
       <c r="O11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="P11" s="4" t="s">
+      <c r="P11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="Q11" s="4" t="s">
+      <c r="Q11" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="R11" s="4" t="s">
+      <c r="R11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="S11" s="4" t="s">
+      <c r="S11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="T11" s="0"/>
-      <c r="U11" s="0"/>
-      <c r="V11" s="0"/>
-      <c r="W11" s="0"/>
-      <c r="X11" s="0"/>
+      <c r="T11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="L12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="M12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="N12" s="4" t="s">
-        <v>53</v>
+      <c r="N12" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>36</v>
@@ -1460,64 +1476,66 @@
       <c r="Q12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="R12" s="4" t="s">
+      <c r="R12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="S12" s="4" t="s">
+      <c r="S12" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="T12" s="4" t="s">
+      <c r="T12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="U12" s="4" t="s">
+      <c r="U12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="V12" s="0"/>
-      <c r="W12" s="0"/>
-      <c r="X12" s="0"/>
+      <c r="V12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="K13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="L13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="M13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="N13" s="4" t="s">
-        <v>53</v>
+      <c r="N13" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>36</v>
@@ -1525,68 +1543,70 @@
       <c r="P13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Q13" s="4" t="s">
+      <c r="Q13" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="R13" s="4" t="s">
+      <c r="R13" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="S13" s="4" t="s">
+      <c r="S13" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="T13" s="4" t="s">
+      <c r="T13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="U13" s="0"/>
-      <c r="V13" s="0"/>
-      <c r="W13" s="0"/>
-      <c r="X13" s="0"/>
+      <c r="U13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="L14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="M14" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="N14" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="O14" s="4" t="s">
-        <v>57</v>
+      <c r="N14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>36</v>
@@ -1597,66 +1617,68 @@
       <c r="R14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="S14" s="4" t="s">
+      <c r="S14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="T14" s="4" t="s">
+      <c r="T14" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="U14" s="4" t="s">
+      <c r="U14" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="V14" s="4" t="s">
+      <c r="V14" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="W14" s="0"/>
-      <c r="X14" s="0"/>
+      <c r="W14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="X14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I15" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="K15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="L15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M15" s="2" t="s">
+      <c r="M15" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="N15" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="O15" s="4" t="s">
-        <v>57</v>
+      <c r="N15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>36</v>
@@ -1664,70 +1686,72 @@
       <c r="Q15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="R15" s="4" t="s">
+      <c r="R15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="S15" s="4" t="s">
+      <c r="S15" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="T15" s="4" t="s">
+      <c r="T15" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="U15" s="4" t="s">
+      <c r="U15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="V15" s="0"/>
-      <c r="W15" s="0"/>
-      <c r="X15" s="0"/>
+      <c r="V15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="J16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="K16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="L16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M16" s="2" t="s">
+      <c r="M16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="N16" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="O16" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="P16" s="4" t="s">
-        <v>53</v>
+      <c r="N16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="Q16" s="1" t="s">
         <v>36</v>
@@ -1738,68 +1762,70 @@
       <c r="S16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="T16" s="4" t="s">
+      <c r="T16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="U16" s="4" t="s">
+      <c r="U16" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="V16" s="4" t="s">
+      <c r="V16" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="W16" s="4" t="s">
+      <c r="W16" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="X16" s="0"/>
+      <c r="X16" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="J17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="K17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="L17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="M17" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="N17" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="O17" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="P17" s="4" t="s">
-        <v>53</v>
+      <c r="N17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="Q17" s="1" t="s">
         <v>36</v>
@@ -1807,61 +1833,76 @@
       <c r="R17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="S17" s="4" t="s">
+      <c r="S17" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="T17" s="4" t="s">
+      <c r="T17" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="U17" s="4" t="s">
+      <c r="U17" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="V17" s="4" t="s">
+      <c r="V17" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="W17" s="0"/>
-      <c r="X17" s="0"/>
+      <c r="W17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="X17" s="2"/>
+    </row>
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S24" s="0"/>
+      <c r="T24" s="0"/>
+      <c r="U24" s="0"/>
+      <c r="V24" s="0"/>
+      <c r="W24" s="0"/>
+    </row>
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S25" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M27" s="0"/>
-      <c r="N27" s="0"/>
-      <c r="O27" s="0"/>
-      <c r="P27" s="0"/>
-      <c r="Q27" s="0"/>
-      <c r="R27" s="0"/>
-      <c r="S27" s="0"/>
+      <c r="M27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M28" s="0"/>
-      <c r="N28" s="0"/>
-      <c r="O28" s="0"/>
-      <c r="P28" s="0"/>
-      <c r="Q28" s="0"/>
-      <c r="R28" s="0"/>
-      <c r="S28" s="0"/>
+      <c r="M28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M29" s="0"/>
-      <c r="N29" s="0"/>
-      <c r="O29" s="0"/>
-      <c r="P29" s="0"/>
-      <c r="Q29" s="0"/>
-      <c r="R29" s="0"/>
-      <c r="S29" s="0"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M30" s="0"/>
-      <c r="N30" s="0"/>
-      <c r="O30" s="0"/>
-      <c r="P30" s="0"/>
-      <c r="Q30" s="0"/>
-      <c r="R30" s="0"/>
-      <c r="S30" s="0"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N31" s="0"/>
-      <c r="O31" s="0"/>
-      <c r="P31" s="0"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+    </row>
+    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>